<commit_message>
latest version to sascha and stefan
</commit_message>
<xml_diff>
--- a/Literature_overview.xlsx
+++ b/Literature_overview.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20410"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFECB4F-A70C-4495-8061-D96F5992AC87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67479CB-553D-45B9-826B-E79D98416D8C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7478,10 +7478,10 @@
   <dimension ref="A1:CK84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="Q59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AZ2" sqref="AZ2"/>
+      <selection pane="bottomRight" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
scanned through remaining papers
</commit_message>
<xml_diff>
--- a/Literature_overview.xlsx
+++ b/Literature_overview.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAABB30D-FE77-4F0A-9A5D-FB61FE04D317}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6D5534-5D14-4663-A299-0083E9B9F78E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -745,7 +745,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2607" uniqueCount="1230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2677" uniqueCount="1265">
   <si>
     <t>Publication</t>
   </si>
@@ -7242,6 +7242,292 @@
   </si>
   <si>
     <t>human-likeness, robotic</t>
+  </si>
+  <si>
+    <t>Lehner_2022</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lehner, K., Ziegler, W., &amp; KommPaS Study Group. (2022). Clinical measures of communication limitations in dysarthria assessed through crowdsourcing: Specificity, sensitivity, and retest-reliability. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Clinical Linguistics &amp; Phonetics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>36</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(11), 988-1009.</t>
+    </r>
+  </si>
+  <si>
+    <t>Lehner</t>
+  </si>
+  <si>
+    <t>"It describes to what extent the way someone speaks sounds natural and not irritating, i.e., whether it conforms to the expected standard of unimpaired speech" (page 990)</t>
+  </si>
+  <si>
+    <t>human and manipulated voices to sound robotic</t>
+  </si>
+  <si>
+    <t>discuss listener adaptation effects</t>
+  </si>
+  <si>
+    <t>dysarthic speech and then rated by naive listeners (0 = very unnatural, 100 = natural)</t>
+  </si>
+  <si>
+    <t>assessment of a diagnostic instrument called "KommPaS" through crowdsourcing, good sensitivity, specificity and retest-reliability; naturalness was the most reliable parameter  discriminating between healthy and dysarthric speakers</t>
+  </si>
+  <si>
+    <t>dysarthria; communication limitation; web-based assessment; crowdsourcing; psychometric evaluation</t>
+  </si>
+  <si>
+    <t>Moya-Gale_2024</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Moya-Galé, G., Pagano, G., &amp; Walsh, S. J. (2024). Perceptual consequences of online group speech treatment for individuals with Parkinson’s disease: A pilot study case series. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>International Journal of Speech-Language Pathology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 1-16.</t>
+    </r>
+  </si>
+  <si>
+    <t>Moya-Gale</t>
+  </si>
+  <si>
+    <t>Parkinsons disease</t>
+  </si>
+  <si>
+    <t>After 10-weeks online treatment, naturalness improved (or stayed the same) in three out of 7 speakers</t>
+  </si>
+  <si>
+    <t>"naturalness, which has been defined as the
+degree to which speech “meets the typical patterns in terms of intonation, voice quality, rate, rhythm, and
+intensity, with respect to the syntactic structure of the
+utterance”" (page 2)</t>
+  </si>
+  <si>
+    <t>monopitch</t>
+  </si>
+  <si>
+    <t>rated via visual analog scale</t>
+  </si>
+  <si>
+    <t>intervention study + rating data</t>
+  </si>
+  <si>
+    <t>van_Prooije_2024</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">van Prooije, T., Knuijt, S., Oostveen, J., Kapteijns, K., Vogel, A. P., &amp; van de Warrenburg, B. (2024). Perceptual and Acoustic Analysis of Speech in Spinocerebellar ataxia Type 1. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Cerebellum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>23</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(1), 112-120.</t>
+    </r>
+  </si>
+  <si>
+    <t>spinocerebellar ataxia type 1; speech; dysarthria</t>
+  </si>
+  <si>
+    <t>teletherapy; group treatment; parkinson’s disease; ease of understanding; naturalness; speech severity</t>
+  </si>
+  <si>
+    <t>Spinocerebellar ataxia</t>
+  </si>
+  <si>
+    <t>expert ratings using direct magnitude estimation (DME), anchor was mild disyarthria</t>
+  </si>
+  <si>
+    <t>patients rated as less natural than the healthy controls</t>
+  </si>
+  <si>
+    <t>Liu_2023</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Liu, X., Dong, J., &amp; Jeon, M. (2023). Robots’“Woohoo” and “Argh” Can Enhance Users’ Emotional and Social Perceptions: An Exploratory Study on Non-lexical Vocalizations and Non-linguistic Sounds. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ACM Transactions on Human-Robot Interaction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(4), 1-20.</t>
+    </r>
+  </si>
+  <si>
+    <t>Liu</t>
+  </si>
+  <si>
+    <t>human-centered computing; auditory feedback; computer systems organization; robotic components</t>
+  </si>
+  <si>
+    <t>non-linguistic vocalizations</t>
+  </si>
+  <si>
+    <t>"Participants showed significantly higher emotion recognition accuracy from the natural voice than from other sounds. […] The natural voice also induced higher trust, naturalness, and preference compared to other sounds."</t>
+  </si>
+  <si>
+    <t>Ziereis_2023</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ziereis, A., &amp; Schacht, A. (2023). Validation of scrambling methods for vocal affect bursts. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Behavior Research Methods</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 1-13.</t>
+    </r>
+  </si>
+  <si>
+    <t>Ziereis</t>
+  </si>
+  <si>
+    <t>voice manipulation</t>
   </si>
 </sst>
 </file>
@@ -7397,7 +7683,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -7575,6 +7861,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -7858,13 +8147,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CK89"/>
+  <dimension ref="A1:CK94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Q86" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B90" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z89" sqref="Z89"/>
+      <selection pane="bottomRight" activeCell="U94" sqref="U94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8575,7 +8864,7 @@
       <c r="CJ4" s="2"/>
       <c r="CK4" s="2"/>
     </row>
-    <row r="5" spans="1:89" s="6" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:89" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
         <v>932</v>
       </c>
@@ -9360,7 +9649,7 @@
       <c r="CJ9" s="2"/>
       <c r="CK9" s="2"/>
     </row>
-    <row r="10" spans="1:89" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:89" s="3" customFormat="1" ht="285" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
         <v>950</v>
       </c>
@@ -9496,7 +9785,7 @@
       <c r="CJ10" s="2"/>
       <c r="CK10" s="2"/>
     </row>
-    <row r="11" spans="1:89" s="6" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:89" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>905</v>
       </c>
@@ -9636,7 +9925,7 @@
       <c r="CJ11" s="2"/>
       <c r="CK11" s="2"/>
     </row>
-    <row r="12" spans="1:89" s="4" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:89" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
         <v>905</v>
       </c>
@@ -10290,7 +10579,7 @@
       <c r="CJ15" s="17"/>
       <c r="CK15" s="17"/>
     </row>
-    <row r="16" spans="1:89" s="6" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:89" s="6" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
         <v>951</v>
       </c>
@@ -10596,7 +10885,7 @@
       <c r="CJ17" s="2"/>
       <c r="CK17" s="2"/>
     </row>
-    <row r="18" spans="1:89" s="9" customFormat="1" ht="255" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:89" s="9" customFormat="1" ht="195" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
         <v>894</v>
       </c>
@@ -10775,7 +11064,7 @@
       <c r="CJ18" s="2"/>
       <c r="CK18" s="2"/>
     </row>
-    <row r="19" spans="1:89" s="3" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:89" s="3" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
         <v>928</v>
       </c>
@@ -10936,7 +11225,7 @@
       <c r="CJ19" s="2"/>
       <c r="CK19" s="2"/>
     </row>
-    <row r="20" spans="1:89" s="6" customFormat="1" ht="240" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:89" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="33" t="s">
         <v>914</v>
       </c>
@@ -11869,7 +12158,7 @@
       <c r="CJ25" s="2"/>
       <c r="CK25" s="2"/>
     </row>
-    <row r="26" spans="1:89" s="9" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:89" s="9" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A26" s="35" t="s">
         <v>927</v>
       </c>
@@ -12159,7 +12448,7 @@
       <c r="CJ27" s="2"/>
       <c r="CK27" s="2"/>
     </row>
-    <row r="28" spans="1:89" s="6" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:89" s="6" customFormat="1" ht="255" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
         <v>942</v>
       </c>
@@ -12793,7 +13082,7 @@
       <c r="CJ31" s="2"/>
       <c r="CK31" s="2"/>
     </row>
-    <row r="32" spans="1:89" s="8" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:89" s="8" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A32" s="33" t="s">
         <v>926</v>
       </c>
@@ -13123,7 +13412,7 @@
       <c r="CJ33" s="2"/>
       <c r="CK33" s="2"/>
     </row>
-    <row r="34" spans="1:89" s="9" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:89" s="9" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A34" s="36" t="s">
         <v>900</v>
       </c>
@@ -13810,7 +14099,7 @@
       <c r="CJ37" s="2"/>
       <c r="CK37" s="2"/>
     </row>
-    <row r="38" spans="1:89" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:89" s="6" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A38" s="33" t="s">
         <v>956</v>
       </c>
@@ -14470,7 +14759,7 @@
       <c r="CJ41" s="2"/>
       <c r="CK41" s="2"/>
     </row>
-    <row r="42" spans="1:89" s="12" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:89" s="12" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A42" s="35" t="s">
         <v>918</v>
       </c>
@@ -14661,7 +14950,7 @@
       <c r="CJ42" s="2"/>
       <c r="CK42" s="2"/>
     </row>
-    <row r="43" spans="1:89" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:89" s="9" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A43" s="35" t="s">
         <v>952</v>
       </c>
@@ -14813,7 +15102,7 @@
       <c r="CJ43" s="2"/>
       <c r="CK43" s="2"/>
     </row>
-    <row r="44" spans="1:89" s="6" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:89" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A44" s="35" t="s">
         <v>901</v>
       </c>
@@ -15000,7 +15289,7 @@
       <c r="CJ44" s="2"/>
       <c r="CK44" s="2"/>
     </row>
-    <row r="45" spans="1:89" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:89" s="6" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A45" s="33" t="s">
         <v>880</v>
       </c>
@@ -15157,7 +15446,7 @@
       <c r="CJ45" s="2"/>
       <c r="CK45" s="2"/>
     </row>
-    <row r="46" spans="1:89" s="12" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:89" s="12" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A46" s="33" t="s">
         <v>902</v>
       </c>
@@ -15348,7 +15637,7 @@
       <c r="CJ46" s="2"/>
       <c r="CK46" s="2"/>
     </row>
-    <row r="47" spans="1:89" s="12" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:89" s="12" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A47" s="33" t="s">
         <v>916</v>
       </c>
@@ -15509,7 +15798,7 @@
       <c r="CJ47" s="2"/>
       <c r="CK47" s="2"/>
     </row>
-    <row r="48" spans="1:89" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:89" s="12" customFormat="1" ht="225" x14ac:dyDescent="0.25">
       <c r="A48" s="33" t="s">
         <v>888</v>
       </c>
@@ -15690,7 +15979,7 @@
       <c r="CJ48" s="2"/>
       <c r="CK48" s="2"/>
     </row>
-    <row r="49" spans="1:89" s="12" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:89" s="12" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A49" s="33" t="s">
         <v>925</v>
       </c>
@@ -16176,7 +16465,7 @@
       <c r="CJ51" s="2"/>
       <c r="CK51" s="2"/>
     </row>
-    <row r="52" spans="1:89" s="6" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:89" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A52" s="33" t="s">
         <v>897</v>
       </c>
@@ -16509,7 +16798,7 @@
       <c r="CJ53" s="2"/>
       <c r="CK53" s="2"/>
     </row>
-    <row r="54" spans="1:89" s="9" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:89" s="9" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A54" s="37" t="s">
         <v>947</v>
       </c>
@@ -16814,7 +17103,7 @@
       <c r="CJ55" s="3"/>
       <c r="CK55" s="3"/>
     </row>
-    <row r="56" spans="1:89" s="12" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:89" s="12" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A56" s="33" t="s">
         <v>939</v>
       </c>
@@ -17086,7 +17375,7 @@
       <c r="CJ57" s="2"/>
       <c r="CK57" s="2"/>
     </row>
-    <row r="58" spans="1:89" s="6" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:89" s="6" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A58" s="36" t="s">
         <v>889</v>
       </c>
@@ -17249,7 +17538,7 @@
       <c r="CJ58" s="17"/>
       <c r="CK58" s="17"/>
     </row>
-    <row r="59" spans="1:89" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:89" s="9" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A59" s="33" t="s">
         <v>922</v>
       </c>
@@ -17426,7 +17715,7 @@
       <c r="CJ59" s="2"/>
       <c r="CK59" s="2"/>
     </row>
-    <row r="60" spans="1:89" s="13" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:89" s="13" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A60" s="33" t="s">
         <v>948</v>
       </c>
@@ -17722,7 +18011,7 @@
       <c r="CJ61" s="2"/>
       <c r="CK61" s="2"/>
     </row>
-    <row r="62" spans="1:89" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:89" s="12" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A62" s="34" t="s">
         <v>903</v>
       </c>
@@ -17907,7 +18196,7 @@
       <c r="CJ62" s="2"/>
       <c r="CK62" s="2"/>
     </row>
-    <row r="63" spans="1:89" s="6" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:89" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A63" s="33" t="s">
         <v>923</v>
       </c>
@@ -18344,7 +18633,7 @@
       <c r="CJ65" s="2"/>
       <c r="CK65" s="2"/>
     </row>
-    <row r="66" spans="1:89" s="6" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:89" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="34" t="s">
         <v>882</v>
       </c>
@@ -18501,7 +18790,7 @@
       <c r="CJ66" s="2"/>
       <c r="CK66" s="2"/>
     </row>
-    <row r="67" spans="1:89" s="12" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:89" s="12" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A67" s="33" t="s">
         <v>940</v>
       </c>
@@ -19006,7 +19295,7 @@
       <c r="CJ69" s="2"/>
       <c r="CK69" s="2"/>
     </row>
-    <row r="70" spans="1:89" s="6" customFormat="1" ht="255" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:89" s="6" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A70" s="33" t="s">
         <v>912</v>
       </c>
@@ -19481,7 +19770,7 @@
       <c r="CJ72" s="2"/>
       <c r="CK72" s="2"/>
     </row>
-    <row r="73" spans="1:89" s="6" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:89" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A73" s="53" t="s">
         <v>1179</v>
       </c>
@@ -19620,7 +19909,7 @@
       <c r="CJ73" s="2"/>
       <c r="CK73" s="2"/>
     </row>
-    <row r="74" spans="1:89" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:89" s="6" customFormat="1" ht="195" x14ac:dyDescent="0.25">
       <c r="A74" s="33" t="s">
         <v>890</v>
       </c>
@@ -19787,7 +20076,7 @@
       <c r="CJ74" s="2"/>
       <c r="CK74" s="2"/>
     </row>
-    <row r="75" spans="1:89" s="6" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:89" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A75" s="33" t="s">
         <v>898</v>
       </c>
@@ -19952,7 +20241,7 @@
       <c r="CJ75" s="2"/>
       <c r="CK75" s="2"/>
     </row>
-    <row r="76" spans="1:89" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:89" s="6" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A76" s="33" t="s">
         <v>891</v>
       </c>
@@ -20105,7 +20394,7 @@
       <c r="CJ76" s="2"/>
       <c r="CK76" s="2"/>
     </row>
-    <row r="77" spans="1:89" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:89" s="6" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A77" s="36" t="s">
         <v>949</v>
       </c>
@@ -20228,7 +20517,7 @@
       <c r="CJ77" s="2"/>
       <c r="CK77" s="2"/>
     </row>
-    <row r="78" spans="1:89" s="6" customFormat="1" ht="225" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:89" s="6" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A78" s="33" t="s">
         <v>924</v>
       </c>
@@ -20531,7 +20820,7 @@
       <c r="CJ79" s="2"/>
       <c r="CK79" s="2"/>
     </row>
-    <row r="80" spans="1:89" s="6" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:89" s="6" customFormat="1" ht="195" x14ac:dyDescent="0.25">
       <c r="A80" s="33" t="s">
         <v>945</v>
       </c>
@@ -20962,7 +21251,7 @@
       <c r="CJ82" s="2"/>
       <c r="CK82" s="2"/>
     </row>
-    <row r="83" spans="1:89" s="9" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:89" s="9" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A83" s="34" t="s">
         <v>907</v>
       </c>
@@ -21147,7 +21436,7 @@
       <c r="CJ83" s="2"/>
       <c r="CK83" s="2"/>
     </row>
-    <row r="84" spans="1:89" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:89" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A84" s="35" t="s">
         <v>908</v>
       </c>
@@ -21773,6 +22062,9 @@
       <c r="N89" s="6">
         <v>1</v>
       </c>
+      <c r="O89" s="6" t="s">
+        <v>1234</v>
+      </c>
       <c r="P89" s="6" t="s">
         <v>1229</v>
       </c>
@@ -21821,8 +22113,395 @@
         <v>1225</v>
       </c>
     </row>
+    <row r="90" spans="1:89" s="9" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A90" s="35" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B90" s="60" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>1232</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E90" s="9">
+        <v>2022</v>
+      </c>
+      <c r="F90" s="9" t="s">
+        <v>1182</v>
+      </c>
+      <c r="G90" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="H90" s="9" t="s">
+        <v>1073</v>
+      </c>
+      <c r="I90" s="9">
+        <v>2</v>
+      </c>
+      <c r="J90" s="9" t="s">
+        <v>1233</v>
+      </c>
+      <c r="K90" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="L90" s="9" t="s">
+        <v>1077</v>
+      </c>
+      <c r="M90" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="N90" s="9">
+        <v>0</v>
+      </c>
+      <c r="O90" s="9" t="s">
+        <v>1236</v>
+      </c>
+      <c r="Q90" s="9" t="s">
+        <v>1072</v>
+      </c>
+      <c r="S90" s="9" t="s">
+        <v>1237</v>
+      </c>
+      <c r="V90" s="9" t="s">
+        <v>1235</v>
+      </c>
+      <c r="X90" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y90" s="4"/>
+      <c r="Z90" s="4"/>
+      <c r="AA90" s="4"/>
+      <c r="AB90" s="4"/>
+      <c r="AC90" s="4"/>
+      <c r="AD90" s="4"/>
+      <c r="AE90" s="4"/>
+      <c r="AF90" s="4"/>
+      <c r="AG90" s="4"/>
+      <c r="AH90" s="28"/>
+      <c r="AI90" s="4"/>
+      <c r="AJ90" s="4"/>
+      <c r="AK90" s="28"/>
+      <c r="AL90" s="4"/>
+      <c r="AM90" s="4"/>
+      <c r="AN90" s="28"/>
+      <c r="AO90" s="4"/>
+      <c r="AP90" s="4"/>
+      <c r="AQ90" s="28"/>
+      <c r="AR90" s="4"/>
+      <c r="AS90" s="4"/>
+      <c r="AT90" s="4"/>
+      <c r="AU90" s="4"/>
+      <c r="AV90" s="4"/>
+      <c r="AW90" s="4"/>
+      <c r="AX90" s="4"/>
+      <c r="AZ90" s="9" t="s">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="91" spans="1:89" s="9" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A91" s="35" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B91" s="60" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C91" s="9" t="s">
+        <v>1241</v>
+      </c>
+      <c r="D91" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E91" s="9">
+        <v>2024</v>
+      </c>
+      <c r="F91" s="9" t="s">
+        <v>1182</v>
+      </c>
+      <c r="G91" s="9" t="s">
+        <v>1242</v>
+      </c>
+      <c r="H91" s="9" t="s">
+        <v>1073</v>
+      </c>
+      <c r="I91" s="9">
+        <v>1</v>
+      </c>
+      <c r="J91" s="9" t="s">
+        <v>1244</v>
+      </c>
+      <c r="K91" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="L91" s="9" t="s">
+        <v>1077</v>
+      </c>
+      <c r="M91" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="N91" s="9">
+        <v>0</v>
+      </c>
+      <c r="O91" s="9" t="s">
+        <v>1246</v>
+      </c>
+      <c r="P91" s="9" t="s">
+        <v>1245</v>
+      </c>
+      <c r="Q91" s="9" t="s">
+        <v>1247</v>
+      </c>
+      <c r="R91" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="S91" s="9" t="s">
+        <v>1243</v>
+      </c>
+      <c r="Y91" s="4"/>
+      <c r="Z91" s="4"/>
+      <c r="AA91" s="4"/>
+      <c r="AB91" s="4"/>
+      <c r="AC91" s="4"/>
+      <c r="AD91" s="4"/>
+      <c r="AE91" s="4"/>
+      <c r="AF91" s="4"/>
+      <c r="AG91" s="4"/>
+      <c r="AH91" s="28"/>
+      <c r="AI91" s="4"/>
+      <c r="AJ91" s="4"/>
+      <c r="AK91" s="28"/>
+      <c r="AL91" s="4"/>
+      <c r="AM91" s="4"/>
+      <c r="AN91" s="28"/>
+      <c r="AO91" s="4"/>
+      <c r="AP91" s="4"/>
+      <c r="AQ91" s="28"/>
+      <c r="AR91" s="4"/>
+      <c r="AS91" s="4"/>
+      <c r="AT91" s="4"/>
+      <c r="AU91" s="4"/>
+      <c r="AV91" s="4"/>
+      <c r="AW91" s="4"/>
+      <c r="AX91" s="4"/>
+      <c r="AZ91" s="9" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="92" spans="1:89" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A92" s="35" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B92" s="60" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C92" s="9" t="s">
+        <v>537</v>
+      </c>
+      <c r="D92" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E92" s="9">
+        <v>2024</v>
+      </c>
+      <c r="F92" s="9" t="s">
+        <v>1182</v>
+      </c>
+      <c r="G92" s="9" t="s">
+        <v>1252</v>
+      </c>
+      <c r="H92" s="9" t="s">
+        <v>1073</v>
+      </c>
+      <c r="I92" s="9">
+        <v>1</v>
+      </c>
+      <c r="K92" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="L92" s="9" t="s">
+        <v>1077</v>
+      </c>
+      <c r="M92" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="N92" s="9">
+        <v>0</v>
+      </c>
+      <c r="O92" s="9" t="s">
+        <v>1253</v>
+      </c>
+      <c r="Q92" s="9" t="s">
+        <v>1072</v>
+      </c>
+      <c r="R92" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="S92" s="9" t="s">
+        <v>1254</v>
+      </c>
+      <c r="X92" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y92" s="4"/>
+      <c r="Z92" s="4"/>
+      <c r="AA92" s="4"/>
+      <c r="AB92" s="4"/>
+      <c r="AC92" s="4"/>
+      <c r="AD92" s="4"/>
+      <c r="AE92" s="4"/>
+      <c r="AF92" s="4"/>
+      <c r="AG92" s="4"/>
+      <c r="AH92" s="28"/>
+      <c r="AI92" s="4"/>
+      <c r="AJ92" s="4"/>
+      <c r="AK92" s="28"/>
+      <c r="AL92" s="4"/>
+      <c r="AM92" s="4"/>
+      <c r="AN92" s="28"/>
+      <c r="AO92" s="4"/>
+      <c r="AP92" s="4"/>
+      <c r="AQ92" s="28"/>
+      <c r="AR92" s="4"/>
+      <c r="AS92" s="4"/>
+      <c r="AT92" s="4"/>
+      <c r="AU92" s="4"/>
+      <c r="AV92" s="4"/>
+      <c r="AW92" s="4"/>
+      <c r="AX92" s="4"/>
+      <c r="AZ92" s="9" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="93" spans="1:89" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A93" s="33" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B93" s="58" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>1257</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E93" s="6">
+        <v>2023</v>
+      </c>
+      <c r="F93" s="6" t="s">
+        <v>1182</v>
+      </c>
+      <c r="G93" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H93" s="6" t="s">
+        <v>1070</v>
+      </c>
+      <c r="I93" s="6">
+        <v>2</v>
+      </c>
+      <c r="K93" s="42"/>
+      <c r="M93" s="42"/>
+      <c r="P93" s="6" t="s">
+        <v>568</v>
+      </c>
+      <c r="S93" s="6" t="s">
+        <v>1260</v>
+      </c>
+      <c r="U93" s="6" t="s">
+        <v>1259</v>
+      </c>
+      <c r="Y93" s="13"/>
+      <c r="Z93" s="13"/>
+      <c r="AA93" s="13"/>
+      <c r="AB93" s="13"/>
+      <c r="AC93" s="13"/>
+      <c r="AD93" s="13"/>
+      <c r="AE93" s="13"/>
+      <c r="AF93" s="13"/>
+      <c r="AG93" s="13"/>
+      <c r="AH93" s="25"/>
+      <c r="AI93" s="13"/>
+      <c r="AJ93" s="13"/>
+      <c r="AK93" s="25"/>
+      <c r="AL93" s="13"/>
+      <c r="AM93" s="13"/>
+      <c r="AN93" s="25"/>
+      <c r="AO93" s="13"/>
+      <c r="AP93" s="13"/>
+      <c r="AQ93" s="25"/>
+      <c r="AR93" s="13"/>
+      <c r="AS93" s="13"/>
+      <c r="AT93" s="13"/>
+      <c r="AU93" s="13"/>
+      <c r="AV93" s="13"/>
+      <c r="AW93" s="13"/>
+      <c r="AX93" s="13"/>
+      <c r="AZ93" s="6" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="94" spans="1:89" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A94" s="34" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B94" s="61" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>1263</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E94" s="3">
+        <v>2023</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>1205</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>1264</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>1079</v>
+      </c>
+      <c r="K94" s="44"/>
+      <c r="M94" s="44"/>
+      <c r="U94" s="3" t="s">
+        <v>1259</v>
+      </c>
+      <c r="Y94" s="23"/>
+      <c r="Z94" s="23"/>
+      <c r="AA94" s="23"/>
+      <c r="AB94" s="23"/>
+      <c r="AC94" s="23"/>
+      <c r="AD94" s="23"/>
+      <c r="AE94" s="23"/>
+      <c r="AF94" s="23"/>
+      <c r="AG94" s="23"/>
+      <c r="AH94" s="27"/>
+      <c r="AI94" s="23"/>
+      <c r="AJ94" s="23"/>
+      <c r="AK94" s="27"/>
+      <c r="AL94" s="23"/>
+      <c r="AM94" s="23"/>
+      <c r="AN94" s="27"/>
+      <c r="AO94" s="23"/>
+      <c r="AP94" s="23"/>
+      <c r="AQ94" s="27"/>
+      <c r="AR94" s="23"/>
+      <c r="AS94" s="23"/>
+      <c r="AT94" s="23"/>
+      <c r="AU94" s="23"/>
+      <c r="AV94" s="23"/>
+      <c r="AW94" s="23"/>
+      <c r="AX94" s="23"/>
+    </row>
   </sheetData>
-  <sortState ref="A2:BB86">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:BB86">
     <sortCondition ref="A2:A86"/>
   </sortState>
   <hyperlinks>

</xml_diff>